<commit_message>
PA: Updated Test Suite Prereq PA: Included Structured162Specification.feature
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PEAL3\Downloads\1.6.2\gpconnect-provider-testing-feature-1.6.2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114AFDF8-1511-4B81-8EF2-6178245EA049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488B8B7E-3471-4BEA-9463-3938DD833ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="13920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,14 +19,12 @@
     <sheet name="Practitioner" sheetId="4" r:id="rId4"/>
     <sheet name="Slots" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="130">
   <si>
     <t>Required Organizations and Slots for testing</t>
   </si>
@@ -471,11 +469,17 @@
 Patient deceased date needs to be within access period</t>
   </si>
   <si>
-    <t>Patient 22</t>
-  </si>
-  <si>
-    <t>Deceased patient.
-Patient deceased date needs to be outside of access period</t>
+    <t>Patient 37</t>
+  </si>
+  <si>
+    <t>Patient 38</t>
+  </si>
+  <si>
+    <t>Patient 39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x
+</t>
   </si>
 </sst>
 </file>
@@ -485,7 +489,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -541,6 +545,10 @@
       <color rgb="FF000000"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1142,11 +1150,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB26"/>
+  <dimension ref="A1:AB28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T26" sqref="T26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2606,14 +2614,14 @@
       <c r="B25" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="C25" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="E25" s="29" t="s">
-        <v>22</v>
+      <c r="C25" s="14">
+        <v>0</v>
+      </c>
+      <c r="D25" s="29">
+        <v>0</v>
+      </c>
+      <c r="E25" s="29">
+        <v>0</v>
       </c>
       <c r="F25" s="14" t="s">
         <v>22</v>
@@ -2624,32 +2632,32 @@
       <c r="H25" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="I25" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="J25" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="K25" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="L25" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="M25" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="N25" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="O25" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="P25" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q25" s="22" t="s">
-        <v>22</v>
+      <c r="I25" s="14">
+        <v>0</v>
+      </c>
+      <c r="J25" s="14">
+        <v>0</v>
+      </c>
+      <c r="K25" s="14">
+        <v>0</v>
+      </c>
+      <c r="L25" s="22">
+        <v>0</v>
+      </c>
+      <c r="M25" s="22">
+        <v>0</v>
+      </c>
+      <c r="N25" s="22">
+        <v>0</v>
+      </c>
+      <c r="O25" s="22">
+        <v>0</v>
+      </c>
+      <c r="P25" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="22">
+        <v>0</v>
       </c>
       <c r="R25" s="16" t="s">
         <v>90</v>
@@ -2667,7 +2675,7 @@
       <c r="AA25" s="6"/>
       <c r="AB25" s="6"/>
     </row>
-    <row r="26" spans="2:28" s="31" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B26" s="26" t="s">
         <v>126</v>
       </c>
@@ -2681,13 +2689,13 @@
         <v>22</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H26" s="14" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I26" s="14" t="s">
         <v>22</v>
@@ -2714,25 +2722,123 @@
         <v>22</v>
       </c>
       <c r="Q26" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="R26" s="16" t="s">
-        <v>127</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="R26" s="16"/>
       <c r="S26" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="T26" s="6"/>
-      <c r="U26" s="6"/>
-      <c r="V26" s="6"/>
-      <c r="W26" s="6"/>
-      <c r="X26" s="6"/>
-      <c r="Y26" s="6"/>
-      <c r="Z26" s="6"/>
-      <c r="AA26" s="6"/>
-      <c r="AB26" s="6"/>
+    </row>
+    <row r="27" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B27" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J27" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K27" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="L27" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="M27" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="N27" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="O27" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="P27" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q27" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="R27" s="16"/>
+      <c r="S27" s="26" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="2:28" ht="30" x14ac:dyDescent="0.25">
+      <c r="B28" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J28" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="K28" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="L28" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="M28" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="N28" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="O28" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="P28" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q28" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="R28" s="16"/>
+      <c r="S28" s="26" t="s">
+        <v>128</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>